<commit_message>
ticket 163: agregados campos de contactos del cliente por tipo de contacto, ajustada plantilla de Anexo-2-Comercial.xlsx de orden de servicio de CNT, y correjido transiciones.php por error extraño de identado
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
   <si>
     <t xml:space="preserve">ANEXO 2 COMERCIAL</t>
   </si>
@@ -55,7 +55,32 @@
     <t xml:space="preserve">CONTACTO COMERCIAL:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONC_NOMBRES} ${CON_APELLIDOS}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${CLI_CONTACTO_COMERCIAL_NOMBRES} ${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">APELLIDOS}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TIPO DE NEGOCIO:</t>
@@ -67,7 +92,32 @@
     <t xml:space="preserve">CARGO:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONC_CARGO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CARGO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">RUC:</t>
@@ -79,7 +129,32 @@
     <t xml:space="preserve">TELÉFONO(S):</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONC_TELEFONO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TELEFONO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">REPRESENTANTE LEGAL:</t>
@@ -91,7 +166,34 @@
     <t xml:space="preserve">E-Mail:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONC_CORREO_ELECTRONICO}</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">DIRECCIÓN:</t>
@@ -103,7 +205,49 @@
     <t xml:space="preserve">CONTACTO TÉCNICO:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONT_NOMBRES} ${CON_APELLIDOS}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NOMBRES} ${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">APELLIDOS}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">CIUDAD:</t>
@@ -112,7 +256,32 @@
     <t xml:space="preserve">${CLI_CIUDAD}</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONT_CARGO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CARGO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">PAÍS:</t>
@@ -121,13 +290,65 @@
     <t xml:space="preserve">${CLI_PAIS}</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONT_TELEFONO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_TECNICO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_TELEFONO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${CLI_TELEFONO}</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONT_CORREO_ELECTRONICO}</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">FAX:</t>
@@ -139,19 +360,111 @@
     <t xml:space="preserve">CONTACTO FACTURACIÓN:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONF_NOMBRES} ${CON_APELLIDOS}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NOMBRES} ${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">APELLIDOS}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${CLI_CORREO_ELECTRONICO}</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONF_CARGO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CARGO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TÉRMINOS DEL CONTRATO</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONF_TELEFONO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TELEFONO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">DURACIÓN:</t>
@@ -160,7 +473,34 @@
     <t xml:space="preserve">1 año</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONF_CORREO_ELECTRONICO}</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">COSTO TOTAL DE INSTALACIÓN:</t>
@@ -172,7 +512,7 @@
     <t xml:space="preserve">DIRECCIÓN ENTREGA DE FACTURA:</t>
   </si>
   <si>
-    <t xml:space="preserve">${DIRECCION_ENTREGA_FACTURA}</t>
+    <t xml:space="preserve">${CLI_DIRECCION_CORRESPONDENCIA}</t>
   </si>
   <si>
     <t xml:space="preserve">COSTO MENSUAL DE LOS SERVICIOS</t>
@@ -184,7 +524,7 @@
     <t xml:space="preserve">HORARIO DE ATENCIÓN:</t>
   </si>
   <si>
-    <t xml:space="preserve">${HORARIO_ATENCION}</t>
+    <t xml:space="preserve">${CLI_HORARIO_ATENCION}</t>
   </si>
   <si>
     <t xml:space="preserve">DETALLE DE LOS VALORES AGREGADOS</t>
@@ -196,7 +536,7 @@
     <t xml:space="preserve">HORARIO DE MONITOREO:</t>
   </si>
   <si>
-    <t xml:space="preserve">${HORARIO_MONITOREO}</t>
+    <t xml:space="preserve">${CLI_HORARIO_MONITOREO}</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPCIÓN DE LOS ENLACES CONTRATADOS</t>
@@ -310,10 +650,10 @@
     <t xml:space="preserve">User SIT</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION} ${CONCENTRADOR_LOGIN}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${EXTREMO_UBI_DIRECCION} ${EXTREMO_LOGIN}</t>
+    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${EXTREMO_UBI_DIRECCION}</t>
   </si>
   <si>
     <t xml:space="preserve">${CONTACTO_DESTINO}</t>
@@ -328,32 +668,7 @@
     <t xml:space="preserve">${CAPACIDAD_FACTURADA_KBPS}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CAPACIDAD_FACTURADA_KBPS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}</t>
-    </r>
+    <t xml:space="preserve">99.6%</t>
   </si>
   <si>
     <t xml:space="preserve">24x7x365</t>
@@ -369,9 +684,6 @@
   </si>
   <si>
     <t xml:space="preserve">${PRECIO_CAPACIDAD_FACTURADA}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${PRECIO_INSTALACION_CLIENTE}</t>
   </si>
   <si>
     <t xml:space="preserve">${ID_SERVICIO}</t>
@@ -493,6 +805,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
@@ -506,11 +823,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -758,7 +1070,7 @@
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -766,7 +1078,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="100">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -879,11 +1191,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -919,7 +1231,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -951,7 +1263,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1119,7 +1431,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1139,7 +1451,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="21" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1165,22 +1477,6 @@
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1202,10 +1498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IW71"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S44" activeCellId="0" sqref="S44"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R18" activeCellId="0" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2335,7 +2631,7 @@
         <v>101</v>
       </c>
       <c r="G44" s="59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H44" s="59" t="s">
         <v>63</v>
@@ -2343,8 +2639,8 @@
       <c r="I44" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="J44" s="63" t="n">
-        <v>0.996</v>
+      <c r="J44" s="63" t="s">
+        <v>102</v>
       </c>
       <c r="K44" s="59" t="s">
         <v>103</v>
@@ -2371,11 +2667,11 @@
         <v>107</v>
       </c>
       <c r="S44" s="66" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="T44" s="9"/>
       <c r="U44" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2449,7 +2745,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q48" s="70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R48" s="65" t="n">
         <f aca="false">SUM(R44:R47)</f>
@@ -2460,7 +2756,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q49" s="70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R49" s="65" t="n">
         <f aca="false">R48*0.14</f>
@@ -2471,7 +2767,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q50" s="70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R50" s="65" t="n">
         <f aca="false">SUM(R48:R49)</f>
@@ -2501,7 +2797,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B52" s="54"/>
       <c r="C52" s="54"/>
@@ -2527,26 +2823,26 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B54" s="58"/>
       <c r="C54" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D54" s="58"/>
       <c r="E54" s="58"/>
       <c r="F54" s="75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G54" s="76"/>
       <c r="H54" s="77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I54" s="77"/>
       <c r="J54" s="76"/>
       <c r="K54" s="76"/>
       <c r="L54" s="78" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M54" s="78"/>
       <c r="N54" s="78"/>
@@ -2558,7 +2854,7 @@
       <c r="A55" s="79"/>
       <c r="B55" s="79"/>
       <c r="C55" s="80" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -2670,7 +2966,7 @@
     </row>
     <row r="66" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B66" s="95"/>
       <c r="C66" s="96"/>
@@ -2682,7 +2978,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="95" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B67" s="95"/>
       <c r="N67" s="14"/>
@@ -2697,7 +2993,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="95" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B68" s="95"/>
       <c r="C68" s="97"/>
@@ -2715,7 +3011,7 @@
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="95" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B69" s="95"/>
       <c r="C69" s="97"/>
@@ -2729,270 +3025,18 @@
       <c r="T69" s="99"/>
       <c r="U69" s="99"/>
     </row>
-    <row r="71" s="103" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="100" t="s">
+    <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="101" t="s">
+      <c r="C71" s="31"/>
+      <c r="D71" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C71" s="101"/>
-      <c r="D71" s="101" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" s="101"/>
-      <c r="F71" s="102"/>
-      <c r="G71" s="102"/>
-      <c r="H71" s="102"/>
-      <c r="I71" s="102"/>
-      <c r="J71" s="102"/>
-      <c r="K71" s="102"/>
-      <c r="L71" s="102"/>
-      <c r="M71" s="102"/>
-      <c r="N71" s="102"/>
-      <c r="O71" s="102"/>
-      <c r="P71" s="102"/>
-      <c r="Q71" s="102"/>
-      <c r="R71" s="102"/>
-      <c r="S71" s="102"/>
-      <c r="T71" s="102"/>
-      <c r="U71" s="102"/>
-      <c r="V71" s="102"/>
-      <c r="W71" s="102"/>
-      <c r="X71" s="102"/>
-      <c r="Y71" s="102"/>
-      <c r="Z71" s="102"/>
-      <c r="AA71" s="102"/>
-      <c r="AB71" s="102"/>
-      <c r="AC71" s="102"/>
-      <c r="AD71" s="102"/>
-      <c r="AE71" s="102"/>
-      <c r="AF71" s="102"/>
-      <c r="AG71" s="102"/>
-      <c r="AH71" s="102"/>
-      <c r="AI71" s="102"/>
-      <c r="AJ71" s="102"/>
-      <c r="AK71" s="102"/>
-      <c r="AL71" s="102"/>
-      <c r="AM71" s="102"/>
-      <c r="AN71" s="102"/>
-      <c r="AO71" s="102"/>
-      <c r="AP71" s="102"/>
-      <c r="AQ71" s="102"/>
-      <c r="AR71" s="102"/>
-      <c r="AS71" s="102"/>
-      <c r="AT71" s="102"/>
-      <c r="AU71" s="102"/>
-      <c r="AV71" s="102"/>
-      <c r="AW71" s="102"/>
-      <c r="AX71" s="102"/>
-      <c r="AY71" s="102"/>
-      <c r="AZ71" s="102"/>
-      <c r="BA71" s="102"/>
-      <c r="BB71" s="102"/>
-      <c r="BC71" s="102"/>
-      <c r="BD71" s="102"/>
-      <c r="BE71" s="102"/>
-      <c r="BF71" s="102"/>
-      <c r="BG71" s="102"/>
-      <c r="BH71" s="102"/>
-      <c r="BI71" s="102"/>
-      <c r="BJ71" s="102"/>
-      <c r="BK71" s="102"/>
-      <c r="BL71" s="102"/>
-      <c r="BM71" s="102"/>
-      <c r="BN71" s="102"/>
-      <c r="BO71" s="102"/>
-      <c r="BP71" s="102"/>
-      <c r="BQ71" s="102"/>
-      <c r="BR71" s="102"/>
-      <c r="BS71" s="102"/>
-      <c r="BT71" s="102"/>
-      <c r="BU71" s="102"/>
-      <c r="BV71" s="102"/>
-      <c r="BW71" s="102"/>
-      <c r="BX71" s="102"/>
-      <c r="BY71" s="102"/>
-      <c r="BZ71" s="102"/>
-      <c r="CA71" s="102"/>
-      <c r="CB71" s="102"/>
-      <c r="CC71" s="102"/>
-      <c r="CD71" s="102"/>
-      <c r="CE71" s="102"/>
-      <c r="CF71" s="102"/>
-      <c r="CG71" s="102"/>
-      <c r="CH71" s="102"/>
-      <c r="CI71" s="102"/>
-      <c r="CJ71" s="102"/>
-      <c r="CK71" s="102"/>
-      <c r="CL71" s="102"/>
-      <c r="CM71" s="102"/>
-      <c r="CN71" s="102"/>
-      <c r="CO71" s="102"/>
-      <c r="CP71" s="102"/>
-      <c r="CQ71" s="102"/>
-      <c r="CR71" s="102"/>
-      <c r="CS71" s="102"/>
-      <c r="CT71" s="102"/>
-      <c r="CU71" s="102"/>
-      <c r="CV71" s="102"/>
-      <c r="CW71" s="102"/>
-      <c r="CX71" s="102"/>
-      <c r="CY71" s="102"/>
-      <c r="CZ71" s="102"/>
-      <c r="DA71" s="102"/>
-      <c r="DB71" s="102"/>
-      <c r="DC71" s="102"/>
-      <c r="DD71" s="102"/>
-      <c r="DE71" s="102"/>
-      <c r="DF71" s="102"/>
-      <c r="DG71" s="102"/>
-      <c r="DH71" s="102"/>
-      <c r="DI71" s="102"/>
-      <c r="DJ71" s="102"/>
-      <c r="DK71" s="102"/>
-      <c r="DL71" s="102"/>
-      <c r="DM71" s="102"/>
-      <c r="DN71" s="102"/>
-      <c r="DO71" s="102"/>
-      <c r="DP71" s="102"/>
-      <c r="DQ71" s="102"/>
-      <c r="DR71" s="102"/>
-      <c r="DS71" s="102"/>
-      <c r="DT71" s="102"/>
-      <c r="DU71" s="102"/>
-      <c r="DV71" s="102"/>
-      <c r="DW71" s="102"/>
-      <c r="DX71" s="102"/>
-      <c r="DY71" s="102"/>
-      <c r="DZ71" s="102"/>
-      <c r="EA71" s="102"/>
-      <c r="EB71" s="102"/>
-      <c r="EC71" s="102"/>
-      <c r="ED71" s="102"/>
-      <c r="EE71" s="102"/>
-      <c r="EF71" s="102"/>
-      <c r="EG71" s="102"/>
-      <c r="EH71" s="102"/>
-      <c r="EI71" s="102"/>
-      <c r="EJ71" s="102"/>
-      <c r="EK71" s="102"/>
-      <c r="EL71" s="102"/>
-      <c r="EM71" s="102"/>
-      <c r="EN71" s="102"/>
-      <c r="EO71" s="102"/>
-      <c r="EP71" s="102"/>
-      <c r="EQ71" s="102"/>
-      <c r="ER71" s="102"/>
-      <c r="ES71" s="102"/>
-      <c r="ET71" s="102"/>
-      <c r="EU71" s="102"/>
-      <c r="EV71" s="102"/>
-      <c r="EW71" s="102"/>
-      <c r="EX71" s="102"/>
-      <c r="EY71" s="102"/>
-      <c r="EZ71" s="102"/>
-      <c r="FA71" s="102"/>
-      <c r="FB71" s="102"/>
-      <c r="FC71" s="102"/>
-      <c r="FD71" s="102"/>
-      <c r="FE71" s="102"/>
-      <c r="FF71" s="102"/>
-      <c r="FG71" s="102"/>
-      <c r="FH71" s="102"/>
-      <c r="FI71" s="102"/>
-      <c r="FJ71" s="102"/>
-      <c r="FK71" s="102"/>
-      <c r="FL71" s="102"/>
-      <c r="FM71" s="102"/>
-      <c r="FN71" s="102"/>
-      <c r="FO71" s="102"/>
-      <c r="FP71" s="102"/>
-      <c r="FQ71" s="102"/>
-      <c r="FR71" s="102"/>
-      <c r="FS71" s="102"/>
-      <c r="FT71" s="102"/>
-      <c r="FU71" s="102"/>
-      <c r="FV71" s="102"/>
-      <c r="FW71" s="102"/>
-      <c r="FX71" s="102"/>
-      <c r="FY71" s="102"/>
-      <c r="FZ71" s="102"/>
-      <c r="GA71" s="102"/>
-      <c r="GB71" s="102"/>
-      <c r="GC71" s="102"/>
-      <c r="GD71" s="102"/>
-      <c r="GE71" s="102"/>
-      <c r="GF71" s="102"/>
-      <c r="GG71" s="102"/>
-      <c r="GH71" s="102"/>
-      <c r="GI71" s="102"/>
-      <c r="GJ71" s="102"/>
-      <c r="GK71" s="102"/>
-      <c r="GL71" s="102"/>
-      <c r="GM71" s="102"/>
-      <c r="GN71" s="102"/>
-      <c r="GO71" s="102"/>
-      <c r="GP71" s="102"/>
-      <c r="GQ71" s="102"/>
-      <c r="GR71" s="102"/>
-      <c r="GS71" s="102"/>
-      <c r="GT71" s="102"/>
-      <c r="GU71" s="102"/>
-      <c r="GV71" s="102"/>
-      <c r="GW71" s="102"/>
-      <c r="GX71" s="102"/>
-      <c r="GY71" s="102"/>
-      <c r="GZ71" s="102"/>
-      <c r="HA71" s="102"/>
-      <c r="HB71" s="102"/>
-      <c r="HC71" s="102"/>
-      <c r="HD71" s="102"/>
-      <c r="HE71" s="102"/>
-      <c r="HF71" s="102"/>
-      <c r="HG71" s="102"/>
-      <c r="HH71" s="102"/>
-      <c r="HI71" s="102"/>
-      <c r="HJ71" s="102"/>
-      <c r="HK71" s="102"/>
-      <c r="HL71" s="102"/>
-      <c r="HM71" s="102"/>
-      <c r="HN71" s="102"/>
-      <c r="HO71" s="102"/>
-      <c r="HP71" s="102"/>
-      <c r="HQ71" s="102"/>
-      <c r="HR71" s="102"/>
-      <c r="HS71" s="102"/>
-      <c r="HT71" s="102"/>
-      <c r="HU71" s="102"/>
-      <c r="HV71" s="102"/>
-      <c r="HW71" s="102"/>
-      <c r="HX71" s="102"/>
-      <c r="HY71" s="102"/>
-      <c r="HZ71" s="102"/>
-      <c r="IA71" s="102"/>
-      <c r="IB71" s="102"/>
-      <c r="IC71" s="102"/>
-      <c r="ID71" s="102"/>
-      <c r="IE71" s="102"/>
-      <c r="IF71" s="102"/>
-      <c r="IG71" s="102"/>
-      <c r="IH71" s="102"/>
-      <c r="II71" s="102"/>
-      <c r="IJ71" s="102"/>
-      <c r="IK71" s="102"/>
-      <c r="IL71" s="102"/>
-      <c r="IM71" s="102"/>
-      <c r="IN71" s="102"/>
-      <c r="IO71" s="102"/>
-      <c r="IP71" s="102"/>
-      <c r="IQ71" s="102"/>
-      <c r="IR71" s="102"/>
-      <c r="IS71" s="102"/>
-      <c r="IT71" s="102"/>
-      <c r="IU71" s="102"/>
-      <c r="IV71" s="102"/>
-      <c r="IW71" s="102"/>
+      <c r="E71" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="68">

</xml_diff>

<commit_message>
ajuste de plantilla de orden de servicio CNT: anexo 2 comercial
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -55,22 +55,51 @@
     <t xml:space="preserve">CONTACTO COMERCIAL:</t>
   </si>
   <si>
+    <t xml:space="preserve">${CLI_CONTACTO_COMERCIAL_NOMBRES} ${CLI_CONTACTO_COMERCIAL_APELLIDOS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIPO DE NEGOCIO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${SER_NOMBRE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARGO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_COMERCIAL_CARGO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUC:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_RUC}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELÉFONO(S):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_COMERCIAL_TELEFONO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPRESENTANTE LEGAL:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_REPRESENTANTE_LEGAL_NOMBRE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Mail:</t>
+  </si>
+  <si>
     <r>
       <rPr>
+        <u val="single"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">${CLI_CONTACTO_COMERCIAL_NOMBRES} ${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
+      <t xml:space="preserve">${</t>
     </r>
     <r>
       <rPr>
@@ -79,17 +108,299 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">APELLIDOS}</t>
+      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">TIPO DE NEGOCIO:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${SER_NOMBRE}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARGO:</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECCIÓN:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_REPRESENTANTE_LEGAL_DIRECCION}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTACTO TÉCNICO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_TECNICO_NOMBRES} ${CLI_CONTACTO_TECNICO_APELLIDOS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIUDAD:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CIUDAD}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_TECNICO_CARGO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAÍS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_PAIS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_TECNICO_TELEFONO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_TELEFONO}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FAX:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_FAX}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTACTO FACTURACIÓN:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_ADMINISTRATIVO_NOMBRES} ${CLI_CONTACTO_ADMINISTRATIVO_APELLIDOS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CORREO_ELECTRONICO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_ADMINISTRATIVO_CARGO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TÉRMINOS DEL CONTRATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_ADMINISTRATIVO_TELEFONO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DURACIÓN:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 año</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CLI_CONTACTO_ADMINISTRATIVO_</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">COSTO TOTAL DE INSTALACIÓN:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${PRECIO_INSTALACION}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECCIÓN ENTREGA DE FACTURA:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_DIRECCION_CORRESPONDENCIA}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSTO MENSUAL DE LOS SERVICIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${PRECIO_MENSUAL}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HORARIO DE ATENCIÓN:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_HORARIO_ATENCION}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DETALLE DE LOS VALORES AGREGADOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${DETALLE_VALORES_AGREGADOS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HORARIO DE MONITOREO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_HORARIO_MONITOREO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIPCIÓN DE LOS ENLACES CONTRATADOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compartido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethernet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no compartido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast Eth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10GE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitio Origen (Dirección)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitio Destiono (Dirección)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacto Destino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teléfono Destino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medio de Trasmisión (Ultima Milla)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BW (Kbps)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocidad Mínima Efectiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condición del Canal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nivel de Compartición del canal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponibilid del servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horarios Soporte del Servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiempo respuesta para solución fallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo Router (marca, modelo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo Moden (solo si aplica)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface Punto A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface Punto Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicios Contratados (Datos o Internet)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio Mensual USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio Instalación USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER OG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User SIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${NODO_UBI_DIRECCION}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${CLI_CONTACTO_EN_SITIO_NOMBRES} ${CLI_CONTACTO_EN_SITIO_APELLIDOS}</t>
   </si>
   <si>
     <r>
@@ -107,7 +418,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
+      <t xml:space="preserve">CLI_</t>
     </r>
     <r>
       <rPr>
@@ -116,550 +427,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">CARGO}</t>
+      <t xml:space="preserve">CONTACTO_EN_SITIO_CELULAR}</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RUC:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_RUC}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELÉFONO(S):</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">TELEFONO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">REPRESENTANTE LEGAL:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_REPRESENTANTE_LEGAL_NOMBRE}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E-Mail:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_COMERCIAL_</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">DIRECCIÓN:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_REPRESENTANTE_LEGAL_DIRECCION}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTACTO TÉCNICO:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NOMBRES} ${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">APELLIDOS}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CIUDAD:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_CIUDAD}</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CARGO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">PAÍS:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_PAIS}</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_TECNICO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_TELEFONO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_TELEFONO}</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_TECNICO_</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">FAX:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_FAX}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONTACTO FACTURACIÓN:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NOMBRES} ${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">APELLIDOS}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_CORREO_ELECTRONICO}</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CARGO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">TÉRMINOS DEL CONTRATO</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">TELEFONO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">DURACIÓN:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 año</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CLI_CONTACTO_FACTURACION_</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CORREO_ELECTRONICO}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">COSTO TOTAL DE INSTALACIÓN:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${PRECIO_INSTALACION}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIRECCIÓN ENTREGA DE FACTURA:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_DIRECCION_CORRESPONDENCIA}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSTO MENSUAL DE LOS SERVICIOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${PRECIO_MENSUAL}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HORARIO DE ATENCIÓN:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_HORARIO_ATENCION}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DETALLE DE LOS VALORES AGREGADOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${DETALLE_VALORES_AGREGADOS}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HORARIO DE MONITOREO:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CLI_HORARIO_MONITOREO}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESCRIPCIÓN DE LOS ENLACES CONTRATADOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compartido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethernet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no compartido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2:1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fast Eth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V.35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G.703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10GE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sitio Origen (Dirección)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sitio Destiono (Dirección)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contacto Destino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teléfono Destino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medio de Trasmisión (Ultima Milla)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BW (Kbps)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Velocidad Mínima Efectiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condición del Canal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nivel de Compartición del canal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disponibilid del servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horarios Soporte del Servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo respuesta para solución fallas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo Router (marca, modelo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo Moden (solo si aplica)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interface Punto A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interface Punto Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servicios Contratados (Datos o Internet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precio Mensual USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precio Instalación USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USER OG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User SIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${EXTREMO_UBI_DIRECCION}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${CONTACTO_DESTINO}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${TELEFONO_DESTINO}</t>
   </si>
   <si>
     <t xml:space="preserve">Fibra Optica</t>
@@ -805,11 +574,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
@@ -823,6 +587,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1070,7 +839,7 @@
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1191,11 +960,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1231,7 +1000,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1263,7 +1032,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1431,7 +1200,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1451,7 +1220,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="21" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1500,8 +1269,8 @@
   </sheetPr>
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R18" activeCellId="0" sqref="R18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G11" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
ticket 173: se agregó la firma para OS CNT, en Anexo-2-Comercial.xls
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="130">
   <si>
     <t xml:space="preserve">ANEXO 2 COMERCIAL</t>
   </si>
@@ -466,13 +466,28 @@
     <t xml:space="preserve">CESAR DAVID ANDRADE</t>
   </si>
   <si>
+    <t xml:space="preserve">${CLI_PERSONA_JURIDICA_REPRESENTANTE_LEGAL_NOMBRE}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vicepresidente Ejecutivo</t>
   </si>
   <si>
+    <t xml:space="preserve">${CLI_PERSONA_JURIDICA_REPRESENTANTE_LEGAL_CARGO}
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">ZENIX TELECOMUNICACIONES</t>
   </si>
   <si>
+    <t xml:space="preserve">${CLI_RAZON_SOCIAL}
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">RUC: 1791946928001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUC: ${CLI_RUC}
+</t>
   </si>
   <si>
     <t xml:space="preserve">Adjuntar</t>
@@ -1239,8 +1254,8 @@
   </sheetPr>
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I69" activeCellId="0" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2703,6 +2718,7 @@
       <c r="P60" s="94"/>
       <c r="Q60" s="87"/>
     </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="95" t="s">
         <v>119</v>
@@ -2711,15 +2727,29 @@
       <c r="C66" s="96"/>
       <c r="D66" s="96"/>
       <c r="E66" s="96"/>
+      <c r="I66" s="95" t="s">
+        <v>120</v>
+      </c>
+      <c r="J66" s="95"/>
+      <c r="K66" s="95"/>
+      <c r="L66" s="95"/>
+      <c r="M66" s="95"/>
       <c r="O66" s="14"/>
       <c r="P66" s="14"/>
       <c r="Q66" s="14"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="95" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B67" s="95"/>
+      <c r="I67" s="95" t="s">
+        <v>122</v>
+      </c>
+      <c r="J67" s="95"/>
+      <c r="K67" s="95"/>
+      <c r="L67" s="95"/>
+      <c r="M67" s="95"/>
       <c r="N67" s="14"/>
       <c r="O67" s="14"/>
       <c r="P67" s="14"/>
@@ -2732,12 +2762,19 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="95" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B68" s="95"/>
       <c r="C68" s="97"/>
       <c r="D68" s="97"/>
       <c r="E68" s="97"/>
+      <c r="I68" s="95" t="s">
+        <v>124</v>
+      </c>
+      <c r="J68" s="95"/>
+      <c r="K68" s="95"/>
+      <c r="L68" s="95"/>
+      <c r="M68" s="95"/>
       <c r="N68" s="14"/>
       <c r="O68" s="98"/>
       <c r="P68" s="98"/>
@@ -2750,12 +2787,19 @@
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="95" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B69" s="95"/>
       <c r="C69" s="97"/>
       <c r="D69" s="97"/>
       <c r="E69" s="97"/>
+      <c r="I69" s="95" t="s">
+        <v>126</v>
+      </c>
+      <c r="J69" s="95"/>
+      <c r="K69" s="95"/>
+      <c r="L69" s="95"/>
+      <c r="M69" s="95"/>
       <c r="O69" s="99"/>
       <c r="P69" s="99"/>
       <c r="Q69" s="99"/>
@@ -2766,19 +2810,19 @@
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="74" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E71" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="68">
+  <mergeCells count="72">
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
     <mergeCell ref="A9:S9"/>
@@ -2840,10 +2884,14 @@
     <mergeCell ref="C60:E60"/>
     <mergeCell ref="J60:K60"/>
     <mergeCell ref="A66:B66"/>
+    <mergeCell ref="I66:M66"/>
     <mergeCell ref="A67:B67"/>
+    <mergeCell ref="I67:M67"/>
     <mergeCell ref="A68:B68"/>
+    <mergeCell ref="I68:M68"/>
     <mergeCell ref="O68:U68"/>
     <mergeCell ref="A69:B69"/>
+    <mergeCell ref="I69:M69"/>
     <mergeCell ref="O69:U69"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="D71:E71"/>

</xml_diff>

<commit_message>
ticket 173: quitado Enter en campos de firma recién incluidos en mejora de plantillas
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="129">
   <si>
     <t xml:space="preserve">ANEXO 2 COMERCIAL</t>
   </si>
@@ -472,22 +472,16 @@
     <t xml:space="preserve">Vicepresidente Ejecutivo</t>
   </si>
   <si>
-    <t xml:space="preserve">${CLI_PERSONA_JURIDICA_REPRESENTANTE_LEGAL_CARGO}
-</t>
+    <t xml:space="preserve">${CLI_PERSONA_JURIDICA_REPRESENTANTE_LEGAL_CARGO}</t>
   </si>
   <si>
     <t xml:space="preserve">ZENIX TELECOMUNICACIONES</t>
   </si>
   <si>
-    <t xml:space="preserve">${CLI_RAZON_SOCIAL}
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">RUC: 1791946928001</t>
   </si>
   <si>
-    <t xml:space="preserve">RUC: ${CLI_RUC}
-</t>
+    <t xml:space="preserve">RUC: ${CLI_RUC}</t>
   </si>
   <si>
     <t xml:space="preserve">Adjuntar</t>
@@ -1255,7 +1249,7 @@
   <dimension ref="A1:V71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I69" activeCellId="0" sqref="I69"/>
+      <selection pane="topLeft" activeCell="I66" activeCellId="0" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2769,7 +2763,7 @@
       <c r="D68" s="97"/>
       <c r="E68" s="97"/>
       <c r="I68" s="95" t="s">
-        <v>124</v>
+        <v>9</v>
       </c>
       <c r="J68" s="95"/>
       <c r="K68" s="95"/>
@@ -2787,14 +2781,14 @@
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B69" s="95"/>
       <c r="C69" s="97"/>
       <c r="D69" s="97"/>
       <c r="E69" s="97"/>
       <c r="I69" s="95" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J69" s="95"/>
       <c r="K69" s="95"/>
@@ -2810,14 +2804,14 @@
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="31" t="s">
         <v>127</v>
-      </c>
-      <c r="B71" s="31" t="s">
-        <v>128</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E71" s="31"/>
     </row>

</xml_diff>

<commit_message>
ticket 163: QUemado pais Ecuador y puesta la ciudad del nodo (extremo en datos) en la ciudad del cliente, en OS CNT, plantilla Anexo-2-comercial.xls
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -137,7 +137,7 @@
     <t xml:space="preserve">CIUDAD:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CLI_CIUDAD}</t>
+    <t xml:space="preserve">${NODO_CIU_NOMBRE}</t>
   </si>
   <si>
     <t xml:space="preserve">${CLI_CONTACTO_TECNICO_CARGO}</t>
@@ -146,7 +146,7 @@
     <t xml:space="preserve">PAÍS:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CLI_PAIS}</t>
+    <t xml:space="preserve">Ecuador</t>
   </si>
   <si>
     <t xml:space="preserve">${CLI_CONTACTO_TECNICO_TELEFONO}</t>
@@ -1248,8 +1248,8 @@
   </sheetPr>
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I66" activeCellId="0" sqref="I66"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
ticket 171: ajustada plantilla de archivo de incremento claro, agregado secuencial de paso
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="134">
   <si>
     <t xml:space="preserve">ANEXO 2 COMERCIAL</t>
   </si>
@@ -430,16 +430,31 @@
     <t xml:space="preserve">${PRECIO_CAPACIDAD_FACTURADA}</t>
   </si>
   <si>
-    <t xml:space="preserve">${ID_SERVICIO}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Subtotal </t>
   </si>
   <si>
+    <t xml:space="preserve">${COSTO_CAPACIDAD_SOLICITADA}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${NODO_NOD_COSTO_INSTALACION_CLIENTE}</t>
+  </si>
+  <si>
     <t xml:space="preserve">IVA 12%</t>
   </si>
   <si>
+    <t xml:space="preserve">${IVA_MENSUAL_SOLICITADO_COSTO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${IVA_INSTALACION}</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${TOTAL_MENSUAL_SOLICITADO_COSTO}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${TOTAL_INSTALACION}</t>
   </si>
   <si>
     <t xml:space="preserve">ESCALAMIENTO DEL CLIENTE</t>
@@ -1088,15 +1103,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="172" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="172" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1248,8 +1263,8 @@
   </sheetPr>
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I19" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S50" activeCellId="0" sqref="S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2414,19 +2429,17 @@
       <c r="R44" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="S44" s="66" t="s">
+      <c r="S44" s="65" t="s">
         <v>48</v>
       </c>
       <c r="T44" s="9"/>
-      <c r="U44" s="9" t="s">
-        <v>108</v>
-      </c>
+      <c r="U44" s="9"/>
     </row>
     <row r="45" s="1" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="59"/>
       <c r="B45" s="60"/>
       <c r="C45" s="60"/>
-      <c r="D45" s="67"/>
+      <c r="D45" s="66"/>
       <c r="E45" s="59"/>
       <c r="F45" s="59"/>
       <c r="G45" s="59"/>
@@ -2440,8 +2453,8 @@
       <c r="O45" s="59"/>
       <c r="P45" s="59"/>
       <c r="Q45" s="64"/>
-      <c r="R45" s="65"/>
-      <c r="S45" s="66"/>
+      <c r="R45" s="67"/>
+      <c r="S45" s="65"/>
       <c r="T45" s="9"/>
       <c r="U45" s="9"/>
     </row>
@@ -2449,7 +2462,7 @@
       <c r="A46" s="59"/>
       <c r="B46" s="60"/>
       <c r="C46" s="60"/>
-      <c r="D46" s="67"/>
+      <c r="D46" s="66"/>
       <c r="E46" s="59"/>
       <c r="F46" s="59"/>
       <c r="G46" s="59"/>
@@ -2463,7 +2476,7 @@
       <c r="O46" s="59"/>
       <c r="P46" s="59"/>
       <c r="Q46" s="64"/>
-      <c r="R46" s="65"/>
+      <c r="R46" s="67"/>
       <c r="S46" s="68"/>
       <c r="T46" s="9"/>
       <c r="U46" s="69"/>
@@ -2486,42 +2499,45 @@
       <c r="O47" s="59"/>
       <c r="P47" s="59"/>
       <c r="Q47" s="64"/>
-      <c r="R47" s="65"/>
+      <c r="R47" s="67"/>
       <c r="S47" s="68"/>
       <c r="T47" s="9"/>
       <c r="U47" s="69"/>
     </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="56.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q48" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="R48" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="R48" s="65" t="n">
-        <f aca="false">SUM(R44:R47)</f>
-        <v>0</v>
-      </c>
-      <c r="S48" s="66"/>
+      <c r="S48" s="65" t="s">
+        <v>110</v>
+      </c>
       <c r="T48" s="45"/>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="34.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q49" s="70" t="s">
-        <v>110</v>
-      </c>
-      <c r="R49" s="65" t="n">
-        <f aca="false">R48*0.14</f>
-        <v>0</v>
-      </c>
-      <c r="S49" s="66"/>
+        <v>111</v>
+      </c>
+      <c r="R49" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="S49" s="65" t="s">
+        <v>113</v>
+      </c>
       <c r="T49" s="45"/>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="34.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q50" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="R50" s="65" t="n">
-        <f aca="false">SUM(R48:R49)</f>
-        <v>0</v>
-      </c>
-      <c r="S50" s="66"/>
+        <v>114</v>
+      </c>
+      <c r="R50" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="S50" s="65" t="s">
+        <v>116</v>
+      </c>
       <c r="T50" s="45"/>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2545,7 +2561,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="54" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B52" s="54"/>
       <c r="C52" s="54"/>
@@ -2571,26 +2587,26 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="58" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B54" s="58"/>
       <c r="C54" s="58" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D54" s="58"/>
       <c r="E54" s="58"/>
       <c r="F54" s="75" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="G54" s="76"/>
       <c r="H54" s="77" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="I54" s="77"/>
       <c r="J54" s="76"/>
       <c r="K54" s="76"/>
       <c r="L54" s="78" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="M54" s="78"/>
       <c r="N54" s="78"/>
@@ -2602,7 +2618,7 @@
       <c r="A55" s="79"/>
       <c r="B55" s="79"/>
       <c r="C55" s="80" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -2715,14 +2731,14 @@
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="95" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B66" s="95"/>
       <c r="C66" s="96"/>
       <c r="D66" s="96"/>
       <c r="E66" s="96"/>
       <c r="I66" s="95" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="J66" s="95"/>
       <c r="K66" s="95"/>
@@ -2734,11 +2750,11 @@
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="95" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B67" s="95"/>
       <c r="I67" s="95" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="J67" s="95"/>
       <c r="K67" s="95"/>
@@ -2756,7 +2772,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="95" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B68" s="95"/>
       <c r="C68" s="97"/>
@@ -2781,14 +2797,14 @@
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="95" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B69" s="95"/>
       <c r="C69" s="97"/>
       <c r="D69" s="97"/>
       <c r="E69" s="97"/>
       <c r="I69" s="95" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="J69" s="95"/>
       <c r="K69" s="95"/>
@@ -2804,14 +2820,14 @@
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="74" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E71" s="31"/>
     </row>

</xml_diff>

<commit_message>
ticket 176: agregadas llamadas AJAX a combos SELECT2 en proceso.php
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
   <si>
     <t xml:space="preserve">ANEXO 2 COMERCIAL</t>
   </si>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">DIRECCIÓN:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CLI_REPRESENTANTE_LEGAL_DIRECCION}</t>
+    <t xml:space="preserve">${CLI_DIRECCION_CORRESPONDENCIA}</t>
   </si>
   <si>
     <t xml:space="preserve">CONTACTO TÉCNICO:</t>
@@ -198,7 +198,7 @@
     <t xml:space="preserve">${CLI_CONTACTO_ADMINISTRATIVO_NOMBRES} ${CLI_CONTACTO_ADMINISTRATIVO_APELLIDOS}</t>
   </si>
   <si>
-    <t xml:space="preserve">${CLI_CORREO_ELECTRONICO}</t>
+    <t xml:space="preserve">${CLI_REPRESENTANTE_LEGAL_EMAIL}</t>
   </si>
   <si>
     <t xml:space="preserve">${CLI_CONTACTO_ADMINISTRATIVO_CARGO}</t>
@@ -256,9 +256,6 @@
     <t xml:space="preserve">DIRECCIÓN ENTREGA DE FACTURA:</t>
   </si>
   <si>
-    <t xml:space="preserve">${CLI_DIRECCION_CORRESPONDENCIA}</t>
-  </si>
-  <si>
     <t xml:space="preserve">COSTO MENSUAL DE LOS SERVICIOS</t>
   </si>
   <si>
@@ -523,7 +520,7 @@
     <numFmt numFmtId="171" formatCode="0.00\ %"/>
     <numFmt numFmtId="172" formatCode="&quot;$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -586,6 +583,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -994,7 +996,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1263,8 +1265,8 @@
   </sheetPr>
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I19" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S50" activeCellId="0" sqref="S50"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -1896,7 +1898,7 @@
         <v>49</v>
       </c>
       <c r="R24" s="46" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="S24" s="46"/>
       <c r="T24" s="46"/>
@@ -1904,10 +1906,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="44" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>52</v>
       </c>
       <c r="C25" s="44"/>
       <c r="D25" s="45"/>
@@ -1924,10 +1926,10 @@
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R25" s="47" t="s">
         <v>53</v>
-      </c>
-      <c r="R25" s="47" t="s">
-        <v>54</v>
       </c>
       <c r="S25" s="47"/>
       <c r="T25" s="47"/>
@@ -1935,10 +1937,10 @@
     </row>
     <row r="26" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="49" t="s">
         <v>55</v>
-      </c>
-      <c r="B26" s="49" t="s">
-        <v>56</v>
       </c>
       <c r="C26" s="49"/>
       <c r="D26" s="50"/>
@@ -1955,10 +1957,10 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="R26" s="51" t="s">
         <v>57</v>
-      </c>
-      <c r="R26" s="51" t="s">
-        <v>58</v>
       </c>
       <c r="S26" s="51"/>
       <c r="T26" s="51"/>
@@ -1986,7 +1988,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="54"/>
       <c r="C28" s="54"/>
@@ -2039,16 +2041,16 @@
       <c r="F30" s="55"/>
       <c r="G30" s="55"/>
       <c r="H30" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="I30" s="56" t="s">
         <v>60</v>
-      </c>
-      <c r="I30" s="56" t="s">
-        <v>61</v>
       </c>
       <c r="J30" s="55"/>
       <c r="K30" s="55"/>
       <c r="L30" s="55"/>
       <c r="O30" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P30" s="55"/>
       <c r="Q30" s="55"/>
@@ -2064,16 +2066,16 @@
       <c r="F31" s="55"/>
       <c r="G31" s="55"/>
       <c r="H31" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="I31" s="56" t="s">
         <v>63</v>
-      </c>
-      <c r="I31" s="56" t="s">
-        <v>64</v>
       </c>
       <c r="J31" s="55"/>
       <c r="K31" s="55"/>
       <c r="L31" s="55"/>
       <c r="O31" s="56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P31" s="55"/>
       <c r="Q31" s="55"/>
@@ -2094,7 +2096,7 @@
       <c r="K32" s="55"/>
       <c r="L32" s="55"/>
       <c r="O32" s="56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P32" s="55"/>
       <c r="Q32" s="55"/>
@@ -2115,7 +2117,7 @@
       <c r="K33" s="55"/>
       <c r="L33" s="55"/>
       <c r="O33" s="56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P33" s="55"/>
       <c r="Q33" s="55"/>
@@ -2136,7 +2138,7 @@
       <c r="K34" s="55"/>
       <c r="L34" s="55"/>
       <c r="O34" s="56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P34" s="55"/>
       <c r="Q34" s="55"/>
@@ -2157,7 +2159,7 @@
       <c r="K35" s="55"/>
       <c r="L35" s="55"/>
       <c r="O35" s="56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P35" s="55"/>
       <c r="Q35" s="55"/>
@@ -2178,7 +2180,7 @@
       <c r="K36" s="55"/>
       <c r="L36" s="55"/>
       <c r="O36" s="56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P36" s="55"/>
       <c r="Q36" s="55"/>
@@ -2199,7 +2201,7 @@
       <c r="K37" s="55"/>
       <c r="L37" s="55"/>
       <c r="O37" s="56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P37" s="55"/>
       <c r="Q37" s="55"/>
@@ -2220,7 +2222,7 @@
       <c r="K38" s="55"/>
       <c r="L38" s="55"/>
       <c r="O38" s="56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P38" s="55"/>
       <c r="Q38" s="55"/>
@@ -2241,7 +2243,7 @@
       <c r="K39" s="55"/>
       <c r="L39" s="55"/>
       <c r="O39" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P39" s="55"/>
       <c r="Q39" s="55"/>
@@ -2262,7 +2264,7 @@
       <c r="K40" s="55"/>
       <c r="L40" s="55"/>
       <c r="O40" s="56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P40" s="55"/>
       <c r="Q40" s="55"/>
@@ -2311,123 +2313,123 @@
     </row>
     <row r="43" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="57" t="s">
+      <c r="C43" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="D43" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="E43" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="E43" s="58" t="s">
+      <c r="F43" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="58" t="s">
+      <c r="G43" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="G43" s="58" t="s">
+      <c r="H43" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="H43" s="58" t="s">
+      <c r="I43" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="I43" s="58" t="s">
+      <c r="J43" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="J43" s="58" t="s">
+      <c r="K43" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="K43" s="58" t="s">
+      <c r="L43" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="L43" s="58" t="s">
+      <c r="M43" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="M43" s="58" t="s">
+      <c r="N43" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="N43" s="58" t="s">
+      <c r="O43" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="O43" s="58" t="s">
+      <c r="P43" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="P43" s="58" t="s">
+      <c r="Q43" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="Q43" s="58" t="s">
+      <c r="R43" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="R43" s="58" t="s">
+      <c r="S43" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="S43" s="58" t="s">
+      <c r="T43" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="T43" s="58" t="s">
+      <c r="U43" s="58" t="s">
         <v>94</v>
-      </c>
-      <c r="U43" s="58" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="true" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="60" t="s">
+      <c r="C44" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="D44" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="61" t="s">
+      <c r="E44" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="E44" s="59" t="s">
+      <c r="F44" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="F44" s="62" t="s">
+      <c r="G44" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="H44" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="I44" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="J44" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="G44" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="H44" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="I44" s="59" t="s">
+      <c r="K44" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="L44" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="M44" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="N44" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="O44" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="J44" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="K44" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="L44" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="M44" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="N44" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="O44" s="59" t="s">
-        <v>62</v>
-      </c>
       <c r="P44" s="59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q44" s="64" t="s">
         <v>13</v>
       </c>
       <c r="R44" s="65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S44" s="65" t="s">
         <v>48</v>
@@ -2506,37 +2508,37 @@
     </row>
     <row r="48" customFormat="false" ht="56.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q48" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="R48" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="R48" s="65" t="s">
+      <c r="S48" s="65" t="s">
         <v>109</v>
-      </c>
-      <c r="S48" s="65" t="s">
-        <v>110</v>
       </c>
       <c r="T48" s="45"/>
     </row>
     <row r="49" customFormat="false" ht="34.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q49" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="R49" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="R49" s="65" t="s">
+      <c r="S49" s="65" t="s">
         <v>112</v>
-      </c>
-      <c r="S49" s="65" t="s">
-        <v>113</v>
       </c>
       <c r="T49" s="45"/>
     </row>
     <row r="50" customFormat="false" ht="34.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q50" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="R50" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="R50" s="65" t="s">
+      <c r="S50" s="65" t="s">
         <v>115</v>
-      </c>
-      <c r="S50" s="65" t="s">
-        <v>116</v>
       </c>
       <c r="T50" s="45"/>
     </row>
@@ -2561,7 +2563,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B52" s="54"/>
       <c r="C52" s="54"/>
@@ -2587,26 +2589,26 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B54" s="58"/>
       <c r="C54" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D54" s="58"/>
       <c r="E54" s="58"/>
       <c r="F54" s="75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G54" s="76"/>
       <c r="H54" s="77" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I54" s="77"/>
       <c r="J54" s="76"/>
       <c r="K54" s="76"/>
       <c r="L54" s="78" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M54" s="78"/>
       <c r="N54" s="78"/>
@@ -2618,7 +2620,7 @@
       <c r="A55" s="79"/>
       <c r="B55" s="79"/>
       <c r="C55" s="80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -2731,14 +2733,14 @@
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="95" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B66" s="95"/>
       <c r="C66" s="96"/>
       <c r="D66" s="96"/>
       <c r="E66" s="96"/>
       <c r="I66" s="95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J66" s="95"/>
       <c r="K66" s="95"/>
@@ -2750,11 +2752,11 @@
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="95" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" s="95"/>
       <c r="I67" s="95" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J67" s="95"/>
       <c r="K67" s="95"/>
@@ -2772,7 +2774,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="95" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B68" s="95"/>
       <c r="C68" s="97"/>
@@ -2797,14 +2799,14 @@
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="95" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B69" s="95"/>
       <c r="C69" s="97"/>
       <c r="D69" s="97"/>
       <c r="E69" s="97"/>
       <c r="I69" s="95" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J69" s="95"/>
       <c r="K69" s="95"/>
@@ -2820,14 +2822,14 @@
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="31" t="s">
         <v>131</v>
-      </c>
-      <c r="B71" s="31" t="s">
-        <v>132</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E71" s="31"/>
     </row>

</xml_diff>

<commit_message>
ticket 193: ajuste en plantilla de orden de servicio
</commit_message>
<xml_diff>
--- a/public/uploads/Anexo-2-Comercial.xlsx
+++ b/public/uploads/Anexo-2-Comercial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="131">
   <si>
     <t xml:space="preserve">ANEXO 2 COMERCIAL</t>
   </si>
@@ -430,16 +430,35 @@
     <t xml:space="preserve">Subtotal </t>
   </si>
   <si>
-    <t xml:space="preserve">${COSTO_CAPACIDAD_SOLICITADA}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${NODO_NOD_COSTO_INSTALACION_CLIENTE}</t>
-  </si>
-  <si>
     <t xml:space="preserve">IVA 12%</t>
   </si>
   <si>
-    <t xml:space="preserve">${IVA_MENSUAL_SOLICITADO_COSTO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${IVA_MENSUAL_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PRECIO_CAPACIDAD_FACTURADA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${IVA_INSTALACION}</t>
@@ -448,7 +467,32 @@
     <t xml:space="preserve">TOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">${TOTAL_MENSUAL_SOLICITADO_COSTO}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">${TOTAL_MENSUAL_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PRECIO_CAPACIDAD_FACTURADA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${TOTAL_INSTALACION}</t>
@@ -996,7 +1040,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1265,8 +1309,8 @@
   </sheetPr>
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F18" colorId="64" zoomScale="48" zoomScaleNormal="48" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R49" activeCellId="0" sqref="R49:R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2506,39 +2550,39 @@
       <c r="T47" s="9"/>
       <c r="U47" s="69"/>
     </row>
-    <row r="48" customFormat="false" ht="56.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="34.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q48" s="70" t="s">
         <v>107</v>
       </c>
       <c r="R48" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="S48" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="T48" s="45"/>
+    </row>
+    <row r="49" customFormat="false" ht="44.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q49" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="S48" s="65" t="s">
+      <c r="R49" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="T48" s="45"/>
-    </row>
-    <row r="49" customFormat="false" ht="34.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q49" s="70" t="s">
+      <c r="S49" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="R49" s="65" t="s">
+      <c r="T49" s="45"/>
+    </row>
+    <row r="50" customFormat="false" ht="44.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q50" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="S49" s="65" t="s">
+      <c r="R50" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="T49" s="45"/>
-    </row>
-    <row r="50" customFormat="false" ht="34.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q50" s="70" t="s">
+      <c r="S50" s="65" t="s">
         <v>113</v>
-      </c>
-      <c r="R50" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="S50" s="65" t="s">
-        <v>115</v>
       </c>
       <c r="T50" s="45"/>
     </row>
@@ -2563,7 +2607,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B52" s="54"/>
       <c r="C52" s="54"/>
@@ -2589,26 +2633,26 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="58" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B54" s="58"/>
       <c r="C54" s="58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D54" s="58"/>
       <c r="E54" s="58"/>
       <c r="F54" s="75" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G54" s="76"/>
       <c r="H54" s="77" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I54" s="77"/>
       <c r="J54" s="76"/>
       <c r="K54" s="76"/>
       <c r="L54" s="78" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M54" s="78"/>
       <c r="N54" s="78"/>
@@ -2620,7 +2664,7 @@
       <c r="A55" s="79"/>
       <c r="B55" s="79"/>
       <c r="C55" s="80" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -2733,14 +2777,14 @@
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="95" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B66" s="95"/>
       <c r="C66" s="96"/>
       <c r="D66" s="96"/>
       <c r="E66" s="96"/>
       <c r="I66" s="95" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J66" s="95"/>
       <c r="K66" s="95"/>
@@ -2752,11 +2796,11 @@
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="95" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B67" s="95"/>
       <c r="I67" s="95" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J67" s="95"/>
       <c r="K67" s="95"/>
@@ -2774,7 +2818,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="95" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B68" s="95"/>
       <c r="C68" s="97"/>
@@ -2799,14 +2843,14 @@
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="95" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B69" s="95"/>
       <c r="C69" s="97"/>
       <c r="D69" s="97"/>
       <c r="E69" s="97"/>
       <c r="I69" s="95" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J69" s="95"/>
       <c r="K69" s="95"/>
@@ -2822,14 +2866,14 @@
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="74" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E71" s="31"/>
     </row>

</xml_diff>